<commit_message>
Sync all changes: add new files, update, and remove deleted files to match local folder state
</commit_message>
<xml_diff>
--- a/data/kb_sheets/testknowledge.xlsx
+++ b/data/kb_sheets/testknowledge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="predisbursal_loan_query_loan_ca" sheetId="1" state="visible" r:id="rId3"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="869">
   <si>
     <t xml:space="preserve">subject</t>
   </si>
@@ -70,19 +70,19 @@
     <t xml:space="preserve">email body</t>
   </si>
   <si>
-    <t xml:space="preserve">IMCreated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMSanctioned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMDisbursed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+Disbursed</t>
+    <t xml:space="preserve">imcreated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imsanctioned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imdisbursed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursed</t>
   </si>
   <si>
     <t xml:space="preserve">Cancel my disbursed</t>
@@ -411,10 +411,10 @@
 We deeply regret the inconvenience caused and thank you for your cooperation in helping us maintain a professional and respectful service environment.</t>
   </si>
   <si>
-    <t xml:space="preserve">IMProcessing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+Listed</t>
+    <t xml:space="preserve">improcessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_listed</t>
   </si>
   <si>
     <t xml:space="preserve">Loan not yet approved</t>
@@ -1009,10 +1009,10 @@
 Team Instamoney</t>
   </si>
   <si>
-    <t xml:space="preserve">IMCreatedBANK_STATEMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMKYCCompleted</t>
+    <t xml:space="preserve">imcreatedbank_statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imkyccompleted</t>
   </si>
   <si>
     <t xml:space="preserve">Bank statement issue</t>
@@ -1400,13 +1400,13 @@
     <t xml:space="preserve">Dear team, I have made a withdrawal from insta money account but funds are yet not credited. It said funds will be available with in 2 hours . Please process it as soon as possible. Regards, Hitesh Rajani 9099803525.</t>
   </si>
   <si>
-    <t xml:space="preserve">IMClosed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+DisbursedBalance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+DisbursedwithoutBalance</t>
+    <t xml:space="preserve">imclosed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursedbalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursedwithoutbalance</t>
   </si>
   <si>
     <t xml:space="preserve">Dear User,
@@ -1500,10 +1500,10 @@
     <t xml:space="preserve">Madhusudan Uthasini : Please close my loan account and update/report in cibil . On Tue, 3 Jun, 2025, 2:52 pm CS InstaMoney, &lt;cs@instamoney.app&gt; wrote: Hello Madhusudan We hope you are doing fine! We would like to inform you that we have not received any response to this email, so we are closing this email for now. Respond back if you wish to communicate further. Best Regards, Customer Support</t>
   </si>
   <si>
-    <t xml:space="preserve">IMDisbursedDelay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+DisbursedDelay</t>
+    <t xml:space="preserve">imdisburseddelay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disburseddelay</t>
   </si>
   <si>
     <t xml:space="preserve">I paid my emi how many times you msg me and remember me 
@@ -2050,7 +2050,7 @@
 Team Instamoney</t>
   </si>
   <si>
-    <t xml:space="preserve">IMDisbursedRegular</t>
+    <t xml:space="preserve">imdisbursedregular</t>
   </si>
   <si>
     <t xml:space="preserve">Need to update in insta money app
@@ -2146,7 +2146,7 @@
 Can you tell my why so? And also let me know how can I option our from the auto debit thing and keep the payment manually.</t>
   </si>
   <si>
-    <t xml:space="preserve">IM</t>
+    <t xml:space="preserve">im</t>
   </si>
   <si>
     <t xml:space="preserve">Dear Customer,
@@ -2159,10 +2159,10 @@
 Team InstaMoney</t>
   </si>
   <si>
-    <t xml:space="preserve">IMDelayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+Delayed</t>
+    <t xml:space="preserve">imdelayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_delayed</t>
   </si>
   <si>
     <t xml:space="preserve">EMI DATE CHANGE</t>
@@ -2333,16 +2333,16 @@
     <t xml:space="preserve">I have Requested to change my EMI date change and why did i recieve emi payment now.</t>
   </si>
   <si>
-    <t xml:space="preserve">IMBank Statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMDisbursedDelayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+DisbursedRegular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IM+DisbursedDelayed</t>
+    <t xml:space="preserve">imbank_statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imdisburseddelayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursedregular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disburseddelayed</t>
   </si>
   <si>
     <t xml:space="preserve">Change my bank account number</t>
@@ -2951,9 +2951,6 @@
     <t xml:space="preserve">Dear sir, Please change my email id.new email id is ramatcr75@gmail.com.If any correspondence please send my personal email id.Do not send my official mail id.please delete my official mail id .please do needful. Regards Ramachandran R</t>
   </si>
   <si>
-    <t xml:space="preserve">IMDsbursedRegular</t>
-  </si>
-  <si>
     <t xml:space="preserve">How can change my mobile number</t>
   </si>
   <si>
@@ -3040,7 +3037,7 @@
     <t xml:space="preserve">Old number:9834570209 New number:- 8141693980 Plz change my mobile number because i hve my bank account in my new number so do it fasttt ....................</t>
   </si>
   <si>
-    <t xml:space="preserve">IM+DisbursedbalanceRegular</t>
+    <t xml:space="preserve">im_disbursedbalanceregular</t>
   </si>
   <si>
     <t xml:space="preserve">Loan closure</t>
@@ -3844,7 +3841,7 @@
 Thanks &amp; Regards</t>
   </si>
   <si>
-    <t xml:space="preserve">IMProfessional Details</t>
+    <t xml:space="preserve">improfessional_details</t>
   </si>
   <si>
     <t xml:space="preserve">Hello </t>
@@ -4025,19 +4022,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Created</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rejected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisbursedRegular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisbursedDelayed</t>
+    <t xml:space="preserve">imrejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_rejected</t>
   </si>
   <si>
     <t xml:space="preserve">Don't msg me</t>
@@ -4115,10 +4109,16 @@
     <t xml:space="preserve">I don't want a loan right now, if Message sends me a lot of loan to get the loan I will report in cyber cell </t>
   </si>
   <si>
-    <t xml:space="preserve">Disbursed30-60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisbursedDelayed90</t>
+    <t xml:space="preserve">imdisbursed30-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imdisburseddelayed90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursed30-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">im_disbursedelayed90</t>
   </si>
   <si>
     <t xml:space="preserve">Request to remove other charges
@@ -4260,9 +4260,6 @@
 No -9897960687</t>
   </si>
   <si>
-    <t xml:space="preserve">Disbursed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remove my PAN and other my personal details from your data base
 </t>
   </si>
@@ -4629,10 +4626,10 @@
 We appreciate your kind words and are happy to know you’re satisfied with the InstaMoney platform. Please feel free to reach out if you need any further support."</t>
   </si>
   <si>
-    <t xml:space="preserve">IMUPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMENach</t>
+    <t xml:space="preserve">imupi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imenach</t>
   </si>
   <si>
     <t xml:space="preserve">For lone mistek</t>
@@ -4662,7 +4659,7 @@
 Team Instamoney</t>
   </si>
   <si>
-    <t xml:space="preserve">IMRegistration Fees</t>
+    <t xml:space="preserve">imregistration_fees</t>
   </si>
   <si>
     <t xml:space="preserve">Hi sir 
@@ -4797,9 +4794,6 @@
 This policy is also outlined in Clause 3.6 of our Terms of Service, which was accepted at the time of application.
 We understand this may be disappointing, but please know that the process followed is transparent and standard across financial services that involve pre-approval assessments.
 If you have any further questions or need assistance, we are here to help.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMRejected</t>
   </si>
   <si>
     <t xml:space="preserve">Loan rejacted</t>
@@ -5587,7 +5581,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="53.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5979,7 +5973,7 @@
   <dimension ref="A2:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="68.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6351,7 +6345,7 @@
   <dimension ref="A2:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="53.3" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6403,7 +6397,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="53.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6581,7 +6575,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="47.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6723,21 +6717,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="M2:N2"/>
+  <dimension ref="A2:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6758,7 +6754,7 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="35.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6830,7 +6826,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="37.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6891,7 +6887,7 @@
       <c r="E4" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>385</v>
       </c>
     </row>
@@ -6925,7 +6921,7 @@
       <c r="C6" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>389</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -7074,7 +7070,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="49.3" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7384,7 +7380,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="43.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7661,7 +7657,7 @@
   <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="39.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7676,7 +7672,7 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7836,18 +7832,18 @@
   </sheetPr>
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="36.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.99"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7858,7 +7854,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>495</v>
+        <v>355</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>409</v>
@@ -7870,234 +7866,234 @@
         <v>411</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>500</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>508</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="F9" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="F12" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>498</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="839.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -8119,7 +8115,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="57.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8141,7 +8137,7 @@
         <v>410</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>411</v>
@@ -8149,232 +8145,232 @@
     </row>
     <row r="3" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>528</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>541</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>575</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="57.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -8428,7 +8424,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="32.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8446,110 +8442,110 @@
     </row>
     <row r="3" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>585</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>590</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>593</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>595</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>597</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>599</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>601</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>603</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="32.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>606</v>
-      </c>
       <c r="C12" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -8634,8 +8630,8 @@
   </sheetPr>
   <dimension ref="A2:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="47.3" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8648,94 +8644,94 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>611</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>620</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="47.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -8756,8 +8752,8 @@
   </sheetPr>
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="60.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8778,13 +8774,13 @@
     </row>
     <row r="3" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>628</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>226</v>
@@ -8798,7 +8794,7 @@
         <v>225</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>226</v>
@@ -8806,13 +8802,13 @@
     </row>
     <row r="5" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>630</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>226</v>
@@ -8820,16 +8816,16 @@
     </row>
     <row r="6" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>633</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8840,19 +8836,19 @@
         <v>231</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>636</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>226</v>
@@ -8860,15 +8856,15 @@
     </row>
     <row r="9" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>638</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>226</v>
       </c>
     </row>
@@ -8877,24 +8873,24 @@
         <v>233</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>640</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>643</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>226</v>
@@ -8902,13 +8898,13 @@
     </row>
     <row r="12" customFormat="false" ht="60.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>645</v>
-      </c>
       <c r="C12" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>226</v>
@@ -8930,15 +8926,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G9"/>
+  <dimension ref="A2:L9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="62.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -8946,116 +8942,182 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="1627" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="F3" s="4" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="827" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>655</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>656</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="677" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>650</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="827" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>656</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="827" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>650</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="827" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>662</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="827" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>650</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -9138,10 +9200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="39.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9154,12 +9216,21 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>649</v>
+        <v>355</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>665</v>
       </c>
     </row>
@@ -9179,6 +9250,15 @@
       <c r="E3" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -9196,6 +9276,15 @@
       <c r="E4" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -9213,6 +9302,15 @@
       <c r="E5" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -9230,6 +9328,15 @@
       <c r="E6" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -9247,6 +9354,15 @@
       <c r="E7" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
@@ -9264,6 +9380,15 @@
       <c r="E8" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -9281,6 +9406,15 @@
       <c r="E9" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -9298,6 +9432,15 @@
       <c r="E10" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
@@ -9315,6 +9458,15 @@
       <c r="E11" s="4" t="s">
         <v>670</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
@@ -9330,6 +9482,15 @@
         <v>669</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>670</v>
       </c>
     </row>
@@ -9349,10 +9510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D15"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="49.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9365,192 +9526,276 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>689</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>692</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>692</v>
+        <v>691</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>695</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>695</v>
+        <v>694</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>698</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>701</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>704</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>707</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>710</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>712</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>715</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>718</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>718</v>
+      <c r="D12" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>721</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>723</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>726</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>725</v>
       </c>
     </row>
   </sheetData>
@@ -9569,10 +9814,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="52.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9587,113 +9832,146 @@
       <c r="C2" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>729</v>
+      <c r="D3" s="4" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>732</v>
+      <c r="D4" s="4" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>734</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>737</v>
+      <c r="D6" s="4" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>739</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>741</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>743</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>744</v>
+      <c r="D9" s="4" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>744</v>
+        <v>743</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>748</v>
+      <c r="D11" s="4" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="52.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>743</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>748</v>
+      <c r="C12" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -9714,8 +9992,8 @@
   </sheetPr>
   <dimension ref="A2:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9727,12 +10005,8 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9753,7 +10027,7 @@
   <dimension ref="A2:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="40.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9766,24 +10040,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="40.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>753</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>754</v>
       </c>
     </row>
   </sheetData>
@@ -9840,9 +10114,9 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="49.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -9850,124 +10124,124 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="1177" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="1202" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="1177" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="1177" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="1227" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>766</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="964.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="1139.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>771</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>772</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>773</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="1314.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>774</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="4" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="1002" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="1102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>778</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>779</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="4" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
   </sheetData>
@@ -10050,10 +10324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="37.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10066,113 +10340,146 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>781</v>
+        <v>645</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>782</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>783</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>784</v>
+      <c r="D3" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>785</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>786</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>787</v>
+      <c r="D4" s="4" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>784</v>
+        <v>782</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>791</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>792</v>
+      <c r="D6" s="4" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>793</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>794</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>795</v>
+      <c r="D7" s="4" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>795</v>
+        <v>793</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>797</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>798</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>799</v>
+      <c r="D9" s="4" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>801</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>802</v>
+      <c r="D10" s="4" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>784</v>
+        <v>782</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>784</v>
+        <v>782</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
   </sheetData>
@@ -10194,7 +10501,7 @@
   <dimension ref="A2:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="45.3" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10455,7 +10762,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
@@ -10471,139 +10778,178 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>781</v>
+        <v>645</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>804</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>807</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>808</v>
+      <c r="D3" s="4" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>810</v>
+        <v>808</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>812</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>813</v>
+      <c r="D5" s="4" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>814</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>815</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>816</v>
+      <c r="D6" s="4" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>818</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>819</v>
+      <c r="D7" s="4" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>821</v>
+        <v>819</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>822</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>823</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>824</v>
+      <c r="D9" s="4" t="s">
+        <v>822</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>821</v>
+        <v>819</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>825</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>828</v>
+      <c r="D11" s="4" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>830</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>831</v>
+      <c r="D12" s="4" t="s">
+        <v>829</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>833</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>834</v>
+      <c r="D13" s="4" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="67.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>835</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>836</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>837</v>
+      <c r="D14" s="4" t="s">
+        <v>835</v>
       </c>
     </row>
   </sheetData>
@@ -10622,10 +10968,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C15"/>
+  <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="37.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10638,146 +10984,188 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>781</v>
+        <v>645</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>839</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>840</v>
+      <c r="D3" s="4" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>842</v>
+        <v>840</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>844</v>
+        <v>842</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>846</v>
+        <v>844</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>848</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>849</v>
+      <c r="D7" s="4" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>851</v>
+        <v>849</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>852</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>853</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>854</v>
+      <c r="D9" s="4" t="s">
+        <v>852</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>855</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>856</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>857</v>
+      <c r="D10" s="4" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>858</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>859</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>860</v>
+      <c r="D11" s="4" t="s">
+        <v>858</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>861</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>862</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>863</v>
+      <c r="D12" s="4" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>864</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>865</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>866</v>
+      <c r="D13" s="4" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>867</v>
+        <v>865</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="37.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>868</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>869</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>870</v>
+      <c r="D15" s="4" t="s">
+        <v>868</v>
       </c>
     </row>
   </sheetData>
@@ -11041,7 +11429,7 @@
   <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="47.95" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11568,8 +11956,8 @@
   </sheetPr>
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="48.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>